<commit_message>
export time + duration + matchid
</commit_message>
<xml_diff>
--- a/lolData.xlsx
+++ b/lolData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Result</t>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Duration</t>
         </is>
       </c>
     </row>
@@ -454,10 +459,11 @@
           <t>OC1_620737042</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2181</v>
       </c>
     </row>
     <row r="3">
@@ -469,10 +475,11 @@
           <t>OC1_615185332</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2090</v>
       </c>
     </row>
     <row r="4">
@@ -484,10 +491,11 @@
           <t>OC1_615179781</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1576</v>
       </c>
     </row>
     <row r="5">
@@ -499,10 +507,11 @@
           <t>OC1_615099142</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1339</v>
       </c>
     </row>
     <row r="6">
@@ -514,10 +523,11 @@
           <t>OC1_615091752</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1959</v>
       </c>
     </row>
   </sheetData>

</xml_diff>